<commit_message>
Add LIS3MDL of the master board and Digikey part number
</commit_message>
<xml_diff>
--- a/ESP32S3/ESP32S3 Carrier/BOM_esp32s3_carrier_2024-01-15.xlsx
+++ b/ESP32S3/ESP32S3 Carrier/BOM_esp32s3_carrier_2024-01-15.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="477">
   <si>
     <t>No.</t>
   </si>
@@ -1325,6 +1325,126 @@
   </si>
   <si>
     <t>https://www.alibaba.com/product-detail/MQ-135-Air-Quality-Detection-Sensor_1600590709708.html?spm=a2700.7724857.0.0.3efc1d24f8tQQM</t>
+  </si>
+  <si>
+    <t>Digikey Part</t>
+  </si>
+  <si>
+    <t>1276-1193-2-ND</t>
+  </si>
+  <si>
+    <t>1276-1001-2-ND</t>
+  </si>
+  <si>
+    <t>1276-1040-2-ND</t>
+  </si>
+  <si>
+    <t>1276-1451-2-ND</t>
+  </si>
+  <si>
+    <t>1276-6807-2-ND</t>
+  </si>
+  <si>
+    <t>13-AC0603KRX7R0BB104TR-ND</t>
+  </si>
+  <si>
+    <t>490-5924-2-ND</t>
+  </si>
+  <si>
+    <t>493-15465-ND</t>
+  </si>
+  <si>
+    <t>709-VPDP302W102K1GV001ETR-ND</t>
+  </si>
+  <si>
+    <t>311-1487-2-ND</t>
+  </si>
+  <si>
+    <t>296-ESDS314DBVRTR-ND</t>
+  </si>
+  <si>
+    <t>SMBJ6.0ALFTR-ND</t>
+  </si>
+  <si>
+    <t>A122867-ND</t>
+  </si>
+  <si>
+    <t>2057-PH1-07-UA-ND</t>
+  </si>
+  <si>
+    <t>445-MPZ2012S601ATD25TR-ND</t>
+  </si>
+  <si>
+    <t>4816-HPC8040NC-330MTR-ND</t>
+  </si>
+  <si>
+    <t>785-1005-2-ND</t>
+  </si>
+  <si>
+    <t>YAG3373TR-ND</t>
+  </si>
+  <si>
+    <t>311-1.00KHRTR-ND</t>
+  </si>
+  <si>
+    <t>311-1.00KLRTR-ND</t>
+  </si>
+  <si>
+    <t>311-10.0KLRTR-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402ZT0R00TR-ND</t>
+  </si>
+  <si>
+    <t>311-2.20KLRTR-ND</t>
+  </si>
+  <si>
+    <t>311-12.1KLRTR-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT24K9TR-ND</t>
+  </si>
+  <si>
+    <t>A129715TR-ND</t>
+  </si>
+  <si>
+    <t>311-4.42KHRTR-ND</t>
+  </si>
+  <si>
+    <t>311-130KHRTR-ND</t>
+  </si>
+  <si>
+    <t>311-10.0KHRTR-ND</t>
+  </si>
+  <si>
+    <t>CSR1206FK30L0TR-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT4R70TR-ND</t>
+  </si>
+  <si>
+    <t>RMCF2512FT4K70TR-ND</t>
+  </si>
+  <si>
+    <t>CR0402-FX-5622GLFTR-ND</t>
+  </si>
+  <si>
+    <t>CR0402-FX-1052GLFTR-ND</t>
+  </si>
+  <si>
+    <t>CAY16-49R9F4LFTR-ND</t>
+  </si>
+  <si>
+    <t>CAT16-222J4LFTR-ND</t>
+  </si>
+  <si>
+    <t>LAN8710A-EZC-TR-ND</t>
+  </si>
+  <si>
+    <t>SMAJ58ALFTR-ND</t>
+  </si>
+  <si>
+    <t>296-46378-2-ND</t>
   </si>
 </sst>
 </file>
@@ -1348,12 +1468,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1369,9 +1495,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1653,18 +1780,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="B51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="14" width="20" customWidth="1"/>
+    <col min="1" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1690,25 +1817,28 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>437</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1734,25 +1864,28 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
+        <v>438</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
       </c>
       <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1778,25 +1911,28 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
+        <v>439</v>
+      </c>
+      <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
         <v>33</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1822,25 +1958,28 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
+        <v>440</v>
+      </c>
+      <c r="J4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
       </c>
       <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
         <v>40</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1866,25 +2005,28 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
+        <v>441</v>
+      </c>
+      <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
       </c>
       <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
         <v>46</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1910,25 +2052,28 @@
         <v>20</v>
       </c>
       <c r="I6" t="s">
+        <v>442</v>
+      </c>
+      <c r="J6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L6" t="s">
         <v>23</v>
       </c>
       <c r="M6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
         <v>51</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1954,69 +2099,72 @@
         <v>56</v>
       </c>
       <c r="I7" t="s">
+        <v>443</v>
+      </c>
+      <c r="J7" t="s">
         <v>57</v>
       </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
       <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
         <v>58</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>59</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>60</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="K8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -2042,25 +2190,28 @@
         <v>75</v>
       </c>
       <c r="I9" t="s">
+        <v>444</v>
+      </c>
+      <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="J9" t="s">
-        <v>22</v>
-      </c>
       <c r="K9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s">
         <v>77</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>78</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>79</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -2086,25 +2237,28 @@
         <v>86</v>
       </c>
       <c r="I10" t="s">
+        <v>445</v>
+      </c>
+      <c r="J10" t="s">
         <v>87</v>
       </c>
-      <c r="J10" t="s">
-        <v>22</v>
-      </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
       </c>
       <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
         <v>88</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -2130,25 +2284,28 @@
         <v>95</v>
       </c>
       <c r="I11" t="s">
+        <v>446</v>
+      </c>
+      <c r="J11" t="s">
         <v>96</v>
       </c>
-      <c r="J11" t="s">
-        <v>22</v>
-      </c>
       <c r="K11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L11" t="s">
         <v>23</v>
       </c>
       <c r="M11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" t="s">
         <v>97</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -2174,69 +2331,72 @@
         <v>56</v>
       </c>
       <c r="I12" t="s">
+        <v>447</v>
+      </c>
+      <c r="J12" t="s">
         <v>103</v>
       </c>
-      <c r="J12" t="s">
-        <v>22</v>
-      </c>
       <c r="K12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L12" t="s">
         <v>23</v>
       </c>
       <c r="M12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
         <v>104</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="J13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -2262,69 +2422,72 @@
         <v>120</v>
       </c>
       <c r="I14" t="s">
+        <v>448</v>
+      </c>
+      <c r="J14" t="s">
         <v>121</v>
       </c>
-      <c r="J14" t="s">
-        <v>22</v>
-      </c>
       <c r="K14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" t="s">
         <v>122</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>123</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>124</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="J15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="K15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -2350,113 +2513,116 @@
         <v>138</v>
       </c>
       <c r="I16" t="s">
+        <v>449</v>
+      </c>
+      <c r="J16" t="s">
         <v>139</v>
       </c>
-      <c r="J16" t="s">
-        <v>22</v>
-      </c>
       <c r="K16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" t="s">
         <v>140</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>141</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>142</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="K17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="K18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -2482,25 +2648,28 @@
         <v>168</v>
       </c>
       <c r="I19" t="s">
+        <v>450</v>
+      </c>
+      <c r="J19" t="s">
         <v>169</v>
       </c>
-      <c r="J19" t="s">
-        <v>22</v>
-      </c>
       <c r="K19" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" t="s">
         <v>170</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>171</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>172</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -2526,25 +2695,28 @@
         <v>178</v>
       </c>
       <c r="I20" t="s">
+        <v>451</v>
+      </c>
+      <c r="J20" t="s">
         <v>179</v>
       </c>
-      <c r="J20" t="s">
-        <v>22</v>
-      </c>
       <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s">
         <v>180</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>181</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>182</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>184</v>
       </c>
@@ -2570,25 +2742,28 @@
         <v>188</v>
       </c>
       <c r="I21" t="s">
+        <v>452</v>
+      </c>
+      <c r="J21" t="s">
         <v>189</v>
       </c>
-      <c r="J21" t="s">
-        <v>22</v>
-      </c>
       <c r="K21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
       </c>
       <c r="M21" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" t="s">
         <v>190</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>192</v>
       </c>
@@ -2614,69 +2789,72 @@
         <v>197</v>
       </c>
       <c r="I22" t="s">
+        <v>453</v>
+      </c>
+      <c r="J22" t="s">
         <v>198</v>
       </c>
-      <c r="J22" t="s">
-        <v>22</v>
-      </c>
       <c r="K22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" t="s">
         <v>199</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>200</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>201</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="J23" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L23" t="s">
-        <v>23</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="K23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>211</v>
       </c>
@@ -2702,25 +2880,28 @@
         <v>215</v>
       </c>
       <c r="I24" t="s">
+        <v>454</v>
+      </c>
+      <c r="J24" t="s">
         <v>216</v>
       </c>
-      <c r="J24" t="s">
-        <v>22</v>
-      </c>
       <c r="K24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s">
         <v>217</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>218</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>219</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>221</v>
       </c>
@@ -2746,25 +2927,28 @@
         <v>56</v>
       </c>
       <c r="I25" t="s">
+        <v>455</v>
+      </c>
+      <c r="J25" t="s">
         <v>226</v>
       </c>
-      <c r="J25" t="s">
-        <v>22</v>
-      </c>
       <c r="K25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
       </c>
       <c r="M25" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" t="s">
         <v>227</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>229</v>
       </c>
@@ -2790,25 +2974,28 @@
         <v>56</v>
       </c>
       <c r="I26" t="s">
+        <v>456</v>
+      </c>
+      <c r="J26" t="s">
         <v>234</v>
       </c>
-      <c r="J26" t="s">
-        <v>22</v>
-      </c>
       <c r="K26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L26" t="s">
         <v>23</v>
       </c>
       <c r="M26" t="s">
+        <v>23</v>
+      </c>
+      <c r="N26" t="s">
         <v>235</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>237</v>
       </c>
@@ -2834,25 +3021,28 @@
         <v>56</v>
       </c>
       <c r="I27" t="s">
+        <v>457</v>
+      </c>
+      <c r="J27" t="s">
         <v>241</v>
       </c>
-      <c r="J27" t="s">
-        <v>22</v>
-      </c>
       <c r="K27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L27" t="s">
         <v>23</v>
       </c>
       <c r="M27" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27" t="s">
         <v>242</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>244</v>
       </c>
@@ -2878,25 +3068,28 @@
         <v>56</v>
       </c>
       <c r="I28" t="s">
+        <v>458</v>
+      </c>
+      <c r="J28" t="s">
         <v>248</v>
       </c>
-      <c r="J28" t="s">
-        <v>22</v>
-      </c>
       <c r="K28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L28" t="s">
         <v>23</v>
       </c>
       <c r="M28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N28" t="s">
         <v>249</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>251</v>
       </c>
@@ -2922,25 +3115,28 @@
         <v>255</v>
       </c>
       <c r="I29" t="s">
+        <v>459</v>
+      </c>
+      <c r="J29" t="s">
         <v>256</v>
       </c>
-      <c r="J29" t="s">
-        <v>22</v>
-      </c>
       <c r="K29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L29" t="s">
         <v>23</v>
       </c>
       <c r="M29" t="s">
+        <v>23</v>
+      </c>
+      <c r="N29" t="s">
         <v>257</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>259</v>
       </c>
@@ -2966,25 +3162,28 @@
         <v>56</v>
       </c>
       <c r="I30" t="s">
+        <v>460</v>
+      </c>
+      <c r="J30" t="s">
         <v>263</v>
       </c>
-      <c r="J30" t="s">
-        <v>22</v>
-      </c>
       <c r="K30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L30" t="s">
         <v>23</v>
       </c>
       <c r="M30" t="s">
+        <v>23</v>
+      </c>
+      <c r="N30" t="s">
         <v>264</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>266</v>
       </c>
@@ -3010,25 +3209,28 @@
         <v>56</v>
       </c>
       <c r="I31" t="s">
+        <v>461</v>
+      </c>
+      <c r="J31" t="s">
         <v>270</v>
       </c>
-      <c r="J31" t="s">
-        <v>22</v>
-      </c>
       <c r="K31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L31" t="s">
         <v>23</v>
       </c>
       <c r="M31" t="s">
+        <v>23</v>
+      </c>
+      <c r="N31" t="s">
         <v>271</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>273</v>
       </c>
@@ -3054,25 +3256,28 @@
         <v>277</v>
       </c>
       <c r="I32" t="s">
+        <v>462</v>
+      </c>
+      <c r="J32" t="s">
         <v>278</v>
       </c>
-      <c r="J32" t="s">
-        <v>22</v>
-      </c>
       <c r="K32" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" t="s">
         <v>279</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>280</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>281</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -3098,25 +3303,28 @@
         <v>277</v>
       </c>
       <c r="I33" t="s">
+        <v>463</v>
+      </c>
+      <c r="J33" t="s">
         <v>287</v>
       </c>
-      <c r="J33" t="s">
-        <v>22</v>
-      </c>
       <c r="K33" t="s">
+        <v>22</v>
+      </c>
+      <c r="L33" t="s">
         <v>288</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>289</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>290</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>292</v>
       </c>
@@ -3142,25 +3350,28 @@
         <v>56</v>
       </c>
       <c r="I34" t="s">
+        <v>464</v>
+      </c>
+      <c r="J34" t="s">
         <v>296</v>
       </c>
-      <c r="J34" t="s">
-        <v>22</v>
-      </c>
       <c r="K34" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" t="s">
         <v>297</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>298</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>299</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>301</v>
       </c>
@@ -3186,25 +3397,28 @@
         <v>56</v>
       </c>
       <c r="I35" t="s">
+        <v>465</v>
+      </c>
+      <c r="J35" t="s">
         <v>305</v>
       </c>
-      <c r="J35" t="s">
-        <v>22</v>
-      </c>
       <c r="K35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L35" t="s">
         <v>23</v>
       </c>
       <c r="M35" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" t="s">
         <v>306</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>308</v>
       </c>
@@ -3230,25 +3444,28 @@
         <v>56</v>
       </c>
       <c r="I36" t="s">
+        <v>466</v>
+      </c>
+      <c r="J36" t="s">
         <v>311</v>
       </c>
-      <c r="J36" t="s">
-        <v>22</v>
-      </c>
       <c r="K36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L36" t="s">
         <v>23</v>
       </c>
       <c r="M36" t="s">
+        <v>23</v>
+      </c>
+      <c r="N36" t="s">
         <v>312</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>314</v>
       </c>
@@ -3274,25 +3491,28 @@
         <v>255</v>
       </c>
       <c r="I37" t="s">
+        <v>467</v>
+      </c>
+      <c r="J37" t="s">
         <v>319</v>
       </c>
-      <c r="J37" t="s">
-        <v>22</v>
-      </c>
       <c r="K37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L37" t="s">
         <v>23</v>
       </c>
       <c r="M37" t="s">
+        <v>23</v>
+      </c>
+      <c r="N37" t="s">
         <v>320</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>322</v>
       </c>
@@ -3318,25 +3538,28 @@
         <v>326</v>
       </c>
       <c r="I38" t="s">
+        <v>468</v>
+      </c>
+      <c r="J38" t="s">
         <v>327</v>
       </c>
-      <c r="J38" t="s">
-        <v>22</v>
-      </c>
       <c r="K38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L38" t="s">
         <v>23</v>
       </c>
       <c r="M38" t="s">
+        <v>23</v>
+      </c>
+      <c r="N38" t="s">
         <v>328</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>330</v>
       </c>
@@ -3362,25 +3585,28 @@
         <v>335</v>
       </c>
       <c r="I39" t="s">
+        <v>469</v>
+      </c>
+      <c r="J39" t="s">
         <v>336</v>
       </c>
-      <c r="J39" t="s">
-        <v>22</v>
-      </c>
       <c r="K39" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" t="s">
         <v>337</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>338</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>339</v>
       </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>341</v>
       </c>
@@ -3406,25 +3632,28 @@
         <v>56</v>
       </c>
       <c r="I40" t="s">
+        <v>470</v>
+      </c>
+      <c r="J40" t="s">
         <v>345</v>
       </c>
-      <c r="J40" t="s">
-        <v>22</v>
-      </c>
       <c r="K40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L40" t="s">
         <v>23</v>
       </c>
       <c r="M40" t="s">
+        <v>23</v>
+      </c>
+      <c r="N40" t="s">
         <v>346</v>
       </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>348</v>
       </c>
@@ -3450,69 +3679,72 @@
         <v>56</v>
       </c>
       <c r="I41" t="s">
+        <v>471</v>
+      </c>
+      <c r="J41" t="s">
         <v>352</v>
       </c>
-      <c r="J41" t="s">
-        <v>22</v>
-      </c>
       <c r="K41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L41" t="s">
         <v>23</v>
       </c>
       <c r="M41" t="s">
+        <v>23</v>
+      </c>
+      <c r="N41" t="s">
         <v>353</v>
       </c>
-      <c r="N41" t="s">
+      <c r="O41" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="F42" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="F42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="J42" t="s">
-        <v>22</v>
-      </c>
-      <c r="K42" t="s">
-        <v>23</v>
-      </c>
-      <c r="L42" t="s">
-        <v>23</v>
-      </c>
-      <c r="M42" t="s">
+      <c r="K42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="N42" t="s">
+      <c r="O42" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>363</v>
       </c>
@@ -3538,25 +3770,28 @@
         <v>368</v>
       </c>
       <c r="I43" t="s">
+        <v>472</v>
+      </c>
+      <c r="J43" t="s">
         <v>369</v>
       </c>
-      <c r="J43" t="s">
-        <v>22</v>
-      </c>
       <c r="K43" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" t="s">
         <v>370</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>371</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>372</v>
       </c>
-      <c r="N43" t="s">
+      <c r="O43" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>374</v>
       </c>
@@ -3582,25 +3817,28 @@
         <v>378</v>
       </c>
       <c r="I44" t="s">
+        <v>473</v>
+      </c>
+      <c r="J44" t="s">
         <v>379</v>
       </c>
-      <c r="J44" t="s">
-        <v>22</v>
-      </c>
       <c r="K44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L44" t="s">
         <v>23</v>
       </c>
       <c r="M44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44" t="s">
         <v>380</v>
       </c>
-      <c r="N44" t="s">
+      <c r="O44" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>382</v>
       </c>
@@ -3625,14 +3863,15 @@
       <c r="H45" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="K45" t="s">
-        <v>23</v>
-      </c>
+      <c r="I45" s="1"/>
       <c r="L45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>385</v>
       </c>
@@ -3658,69 +3897,72 @@
         <v>389</v>
       </c>
       <c r="I46" t="s">
+        <v>474</v>
+      </c>
+      <c r="J46" t="s">
         <v>390</v>
       </c>
-      <c r="J46" t="s">
-        <v>22</v>
-      </c>
       <c r="K46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L46" t="s">
         <v>23</v>
       </c>
       <c r="M46" t="s">
+        <v>23</v>
+      </c>
+      <c r="N46" t="s">
         <v>391</v>
       </c>
-      <c r="N46" t="s">
+      <c r="O46" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F47" t="s">
-        <v>23</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="F47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="J47" t="s">
-        <v>22</v>
-      </c>
-      <c r="K47" t="s">
+      <c r="K47" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M47" t="s">
+      <c r="N47" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="N47" t="s">
+      <c r="O47" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>400</v>
       </c>
@@ -3746,25 +3988,28 @@
         <v>138</v>
       </c>
       <c r="I48" t="s">
+        <v>475</v>
+      </c>
+      <c r="J48" t="s">
         <v>404</v>
       </c>
-      <c r="J48" t="s">
-        <v>22</v>
-      </c>
       <c r="K48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L48" t="s">
         <v>405</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>406</v>
       </c>
-      <c r="M48" t="s">
+      <c r="N48" t="s">
         <v>407</v>
       </c>
-      <c r="N48" t="s">
+      <c r="O48" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>409</v>
       </c>
@@ -3790,113 +4035,116 @@
         <v>120</v>
       </c>
       <c r="I49" t="s">
+        <v>476</v>
+      </c>
+      <c r="J49" t="s">
         <v>413</v>
       </c>
-      <c r="J49" t="s">
-        <v>22</v>
-      </c>
       <c r="K49" t="s">
+        <v>22</v>
+      </c>
+      <c r="L49" t="s">
         <v>414</v>
       </c>
-      <c r="L49" t="s">
+      <c r="M49" t="s">
         <v>415</v>
       </c>
-      <c r="M49" t="s">
+      <c r="N49" t="s">
         <v>414</v>
       </c>
-      <c r="N49" t="s">
+      <c r="O49" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B50" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F50" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" t="s">
+      <c r="F50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="J50" t="s">
-        <v>22</v>
-      </c>
-      <c r="K50" t="s">
+      <c r="K50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L50" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="N50" t="s">
+      <c r="O50" s="2" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="F51" t="s">
-        <v>23</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="F51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="J51" t="s">
-        <v>22</v>
-      </c>
-      <c r="K51" t="s">
+      <c r="K51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L51" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="L51" t="s">
+      <c r="M51" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="M51" t="s">
+      <c r="N51" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="N51" t="s">
+      <c r="O51" s="2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>23</v>
       </c>

</xml_diff>